<commit_message>
AZE aktualisiert, Rev B fertig und Zatl geschickt (27.12.2023, 18:24:21)
</commit_message>
<xml_diff>
--- a/2324_5AHEL_AZE_DA_SumoBots.xlsx
+++ b/2324_5AHEL_AZE_DA_SumoBots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92540BFB-F965-4A2B-A6B9-C0DAC7BE36CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9281EA-B7E5-4ADF-88CD-BB868F951C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="215">
   <si>
     <t>Datum</t>
   </si>
@@ -695,6 +695,9 @@
   </si>
   <si>
     <t>PCB fertiggestellt</t>
+  </si>
+  <si>
+    <t>Infrarotsensoren hinzugefügt, M3-Bohrlöcher mit Masseverbindung eingebunden</t>
   </si>
 </sst>
 </file>
@@ -59225,10 +59228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7A7534-694C-40D9-8751-CE2B801AD914}">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H120" sqref="H120"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -62029,7 +62032,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="34">
         <v>45287</v>
       </c>
@@ -62040,18 +62043,46 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D117" s="35">
-        <v>0.58333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="E117" s="35">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>213</v>
+        <f>D117-C117</f>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F117" s="45" t="s">
+        <v>214</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="H117" s="45" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="36">
+        <v>45287</v>
+      </c>
+      <c r="B118" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" s="37">
+        <v>0.625</v>
+      </c>
+      <c r="D118" s="37">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E118" s="37">
+        <f>D118-C118</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F118" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G118" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H118" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -64217,7 +64248,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
AZE nochmal, hab was vergessen
</commit_message>
<xml_diff>
--- a/2324_5AHEL_AZE_DA_SumoBots.xlsx
+++ b/2324_5AHEL_AZE_DA_SumoBots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9281EA-B7E5-4ADF-88CD-BB868F951C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ECFEB0-625A-43F4-86C0-E5DB3BADF5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="876" firstSheet="2" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AZE" sheetId="12" r:id="rId1"/>
@@ -17608,7 +17608,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60</c:v>
@@ -59230,7 +59230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7A7534-694C-40D9-8751-CE2B801AD914}">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
@@ -64247,8 +64247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BB28D7-011E-4B1C-B663-A596F4715764}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64430,7 +64430,7 @@
         <v>84.1</v>
       </c>
       <c r="F13" s="6">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>